<commit_message>
Casos de uso especifico, aplicativo para leer archivos excel y obtener sus datos
</commit_message>
<xml_diff>
--- a/docs/daily-scrum-meeting-template.xlsx
+++ b/docs/daily-scrum-meeting-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bibliotecas\Escritorio\Proyecto SENA WEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FormaSer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A0FCE8-E33E-47AC-A1E7-7532A07C64A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F41B6D-D015-4D8C-93AC-F24DDAD1DA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
   <si>
     <t>PROJECT MANAGER</t>
   </si>
@@ -130,13 +130,25 @@
     <t>Jhon Alexander Narvadez Lopes</t>
   </si>
   <si>
-    <t>Busqueda y adaptación de diseño</t>
-  </si>
-  <si>
     <t>Diligenciación de formato de requerimientos eiii 830</t>
   </si>
   <si>
-    <t>Login, Register, diagramas</t>
+    <t>Desarrollod de Login, Register, y diagramas UML</t>
+  </si>
+  <si>
+    <t>Casos de uso especifico, aplicativo para leer archivos excel y obtener sus datos</t>
+  </si>
+  <si>
+    <t>Ninguno</t>
+  </si>
+  <si>
+    <t>tablas de casos de uso: Postcondiciones,Extensiones,Inclusiones,Prioridad</t>
+  </si>
+  <si>
+    <t>Busqueda y adaptación de plantilla para el diseño web</t>
+  </si>
+  <si>
+    <t>Diseño y maquetación de la página basdo en los requerimientos</t>
   </si>
 </sst>
 </file>
@@ -369,6 +381,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -389,9 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1198,7 +1210,7 @@
       <c r="C7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="14">
         <v>45390</v>
       </c>
     </row>
@@ -1222,8 +1234,8 @@
   </sheetPr>
   <dimension ref="B6:I20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,21 +1243,23 @@
     <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" customWidth="1"/>
-    <col min="4" max="8" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="8" width="26.28515625" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:9" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="2:9" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:9" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,120 +1288,138 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:9" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="2:9" s="3" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="2:9" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
+    <row r="10" spans="2:9" s="3" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
       <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:9" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+    <row r="12" spans="2:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
+    <row r="13" spans="2:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
       <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+    <row r="15" spans="2:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="2:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -1395,7 +1427,7 @@
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1409,7 +1441,7 @@
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="4" t="s">
         <v>24</v>
       </c>
@@ -1421,7 +1453,7 @@
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="13" t="s">
         <v>25</v>
       </c>
@@ -1466,15 +1498,15 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:8" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:8" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1501,7 +1533,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1514,7 +1546,7 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1525,7 +1557,7 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1536,7 +1568,7 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1549,7 +1581,7 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1560,7 +1592,7 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1571,7 +1603,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1584,7 +1616,7 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1595,7 +1627,7 @@
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1606,7 +1638,7 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1619,7 +1651,7 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
@@ -1630,7 +1662,7 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
@@ -1673,15 +1705,15 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:8" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:8" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1708,7 +1740,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1721,7 +1753,7 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1732,7 +1764,7 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1743,7 +1775,7 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1756,7 +1788,7 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1767,7 +1799,7 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1778,7 +1810,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1791,7 +1823,7 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1802,7 +1834,7 @@
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
@@ -1813,7 +1845,7 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1826,7 +1858,7 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
@@ -1837,7 +1869,7 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
@@ -1880,15 +1912,15 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:8" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:8" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1915,7 +1947,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1928,7 +1960,7 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1939,7 +1971,7 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1950,7 +1982,7 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1963,7 +1995,7 @@
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
@@ -1974,7 +2006,7 @@
       <c r="H13" s="7"/>
     </row>
     <row r="14" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
@@ -1985,7 +2017,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1998,7 +2030,7 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
@@ -2009,7 +2041,7 @@
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
@@ -2020,7 +2052,7 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -2033,7 +2065,7 @@
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="4" t="s">
         <v>11</v>
       </c>
@@ -2044,7 +2076,7 @@
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Validación de primer formato
</commit_message>
<xml_diff>
--- a/docs/daily-scrum-meeting-template.xlsx
+++ b/docs/daily-scrum-meeting-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FormaSer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F41B6D-D015-4D8C-93AC-F24DDAD1DA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E536515-D5F9-49B5-9DC7-706D777A16BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="44">
   <si>
     <t>PROJECT MANAGER</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Diseño y maquetación de la página basdo en los requerimientos</t>
+  </si>
+  <si>
+    <t>Desarrollo de Login y diagramas UML</t>
+  </si>
+  <si>
+    <t>Desarrollo de la aplicación(Lectura de excels y escritura en la base de datos)</t>
+  </si>
+  <si>
+    <t>Desarrollo de funciones de escritura en la base de datos (UPDATE)</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1244,7 @@
   <dimension ref="B6:I20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1308,9 @@
       <c r="E9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -1310,13 +1321,15 @@
         <v>24</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
@@ -1345,7 +1358,9 @@
       <c r="E12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -1391,7 +1406,9 @@
       <c r="E15" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -1408,7 +1425,9 @@
         <v>38</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>

</xml_diff>